<commit_message>
Comparación de recursos en escaleta y greco
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion01/ESCALETA_MA_09_01_CO/ESCALETA_MA_09_01_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion01/ESCALETA_MA_09_01_CO/ESCALETA_MA_09_01_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ARCHIVOS PLANETA. FERNANDA\ESCALETAS\ESCALETA_MA_09_01_CO\ESCALETA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lzambrano\Documents\GitHub\Matematicas\fuentes\contenidos\grado09\guion01\ESCALETA_MA_09_01_CO\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -891,9 +891,6 @@
   </si>
   <si>
     <t>Adaptar y complementar el contenido del recurso del autor MA_09_01_CO_REC120.  Axioma de completitud.</t>
-  </si>
-  <si>
-    <t>Proyecto: estudio del número π</t>
   </si>
   <si>
     <t>Interactivo que presenta aspectos del número π para visualizar y formular situaciones de formas no convencionales</t>
@@ -1163,6 +1160,9 @@
   </si>
   <si>
     <t>Motor que incluye actividades de respuesta abierta del tema Los números reales</t>
+  </si>
+  <si>
+    <t>Competencias: estudio del número π</t>
   </si>
 </sst>
 </file>
@@ -1563,56 +1563,56 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1644,47 +1644,47 @@
     <xf numFmtId="0" fontId="4" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6278,8 +6278,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35:J38"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -6291,14 +6291,14 @@
     <col min="5" max="5" width="22.85546875" style="32" customWidth="1"/>
     <col min="6" max="6" width="25.42578125" style="32" customWidth="1"/>
     <col min="7" max="7" width="30.42578125" style="32" customWidth="1"/>
-    <col min="8" max="8" width="9" style="32" customWidth="1"/>
-    <col min="9" max="9" width="6.28515625" style="32" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="86.140625" style="32" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" style="32" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" style="32" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.7109375" style="42" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.5703125" style="42" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="33.140625" style="32" customWidth="1"/>
+    <col min="8" max="8" width="9" style="32" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="6.28515625" style="32" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="86.140625" style="32" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" style="32" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="32" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="4.7109375" style="42" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="7.5703125" style="42" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="33.140625" style="32" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="12.7109375" style="52" customWidth="1"/>
     <col min="17" max="17" width="8.42578125" style="32" customWidth="1"/>
     <col min="18" max="18" width="6.7109375" style="32" customWidth="1"/>
@@ -6315,62 +6315,62 @@
       <c r="A1" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="77" t="s">
+      <c r="B1" s="67" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="82" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="83" t="s">
+        <v>323</v>
+      </c>
+      <c r="E1" s="85" t="s">
         <v>324</v>
       </c>
-      <c r="E1" s="85" t="s">
+      <c r="F1" s="87" t="s">
         <v>325</v>
       </c>
-      <c r="F1" s="87" t="s">
+      <c r="G1" s="62" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="99" t="s">
+        <v>327</v>
+      </c>
+      <c r="I1" s="99" t="s">
         <v>326</v>
-      </c>
-      <c r="G1" s="67" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="70" t="s">
-        <v>328</v>
-      </c>
-      <c r="I1" s="70" t="s">
-        <v>327</v>
       </c>
       <c r="J1" s="81" t="s">
         <v>6</v>
       </c>
       <c r="K1" s="80" t="s">
-        <v>307</v>
-      </c>
-      <c r="L1" s="67" t="s">
+        <v>306</v>
+      </c>
+      <c r="L1" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="73" t="s">
+      <c r="M1" s="102" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="73"/>
-      <c r="O1" s="72" t="s">
+      <c r="N1" s="102"/>
+      <c r="O1" s="101" t="s">
         <v>199</v>
       </c>
-      <c r="P1" s="62" t="s">
-        <v>329</v>
-      </c>
-      <c r="Q1" s="74" t="s">
+      <c r="P1" s="92" t="s">
+        <v>328</v>
+      </c>
+      <c r="Q1" s="89" t="s">
         <v>121</v>
       </c>
-      <c r="R1" s="76" t="s">
+      <c r="R1" s="91" t="s">
         <v>122</v>
       </c>
-      <c r="S1" s="74" t="s">
+      <c r="S1" s="89" t="s">
         <v>123</v>
       </c>
-      <c r="T1" s="75" t="s">
+      <c r="T1" s="90" t="s">
         <v>124</v>
       </c>
-      <c r="U1" s="74" t="s">
+      <c r="U1" s="89" t="s">
         <v>125</v>
       </c>
       <c r="X1" s="33" t="s">
@@ -6382,30 +6382,30 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="79"/>
-      <c r="B2" s="78"/>
+      <c r="B2" s="69"/>
       <c r="C2" s="82"/>
       <c r="D2" s="84"/>
       <c r="E2" s="86"/>
       <c r="F2" s="88"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="100"/>
+      <c r="I2" s="100"/>
       <c r="J2" s="81"/>
       <c r="K2" s="80"/>
-      <c r="L2" s="67"/>
+      <c r="L2" s="62"/>
       <c r="M2" s="34" t="s">
         <v>126</v>
       </c>
       <c r="N2" s="34" t="s">
         <v>127</v>
       </c>
-      <c r="O2" s="72"/>
-      <c r="P2" s="63"/>
-      <c r="Q2" s="74"/>
-      <c r="R2" s="76"/>
-      <c r="S2" s="74"/>
-      <c r="T2" s="75"/>
-      <c r="U2" s="74"/>
+      <c r="O2" s="101"/>
+      <c r="P2" s="93"/>
+      <c r="Q2" s="89"/>
+      <c r="R2" s="91"/>
+      <c r="S2" s="89"/>
+      <c r="T2" s="90"/>
+      <c r="U2" s="89"/>
       <c r="X2" s="33" t="s">
         <v>206</v>
       </c>
@@ -6429,7 +6429,7 @@
       <c r="E3" s="37"/>
       <c r="F3" s="54"/>
       <c r="G3" s="59" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="H3" s="55">
         <v>1</v>
@@ -6438,7 +6438,7 @@
         <v>207</v>
       </c>
       <c r="J3" s="61" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="K3" s="40" t="s">
         <v>208</v>
@@ -6451,7 +6451,7 @@
       </c>
       <c r="N3" s="34"/>
       <c r="O3" s="58" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="P3" s="51" t="s">
         <v>207</v>
@@ -6516,7 +6516,7 @@
         <v>103</v>
       </c>
       <c r="O4" s="46" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="P4" s="51" t="s">
         <v>207</v>
@@ -6531,7 +6531,7 @@
         <v>270</v>
       </c>
       <c r="T4" s="45" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="U4" s="44" t="s">
         <v>272</v>
@@ -6661,7 +6661,7 @@
         <v>213</v>
       </c>
       <c r="T6" s="45" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="U6" s="44" t="s">
         <v>214</v>
@@ -6691,7 +6691,7 @@
       </c>
       <c r="F7" s="46"/>
       <c r="G7" s="59" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H7" s="55">
         <v>5</v>
@@ -6700,7 +6700,7 @@
         <v>207</v>
       </c>
       <c r="J7" s="61" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="K7" s="40" t="s">
         <v>208</v>
@@ -6754,7 +6754,7 @@
       </c>
       <c r="F8" s="46"/>
       <c r="G8" s="38" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H8" s="55">
         <v>6</v>
@@ -6876,7 +6876,7 @@
       <c r="E10" s="37"/>
       <c r="F10" s="46"/>
       <c r="G10" s="38" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H10" s="55">
         <v>8</v>
@@ -6885,7 +6885,7 @@
         <v>208</v>
       </c>
       <c r="J10" s="61" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="K10" s="40" t="s">
         <v>207</v>
@@ -6907,7 +6907,7 @@
         <v>219</v>
       </c>
       <c r="T10" s="49" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="U10" s="48" t="s">
         <v>228</v>
@@ -6942,7 +6942,7 @@
         <v>208</v>
       </c>
       <c r="J11" s="61" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="K11" s="40" t="s">
         <v>207</v>
@@ -7066,7 +7066,7 @@
         <v>208</v>
       </c>
       <c r="J13" s="61" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="K13" s="40" t="s">
         <v>207</v>
@@ -7118,7 +7118,7 @@
       </c>
       <c r="F14" s="46"/>
       <c r="G14" s="60" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H14" s="55">
         <v>12</v>
@@ -7127,7 +7127,7 @@
         <v>208</v>
       </c>
       <c r="J14" s="61" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="K14" s="40" t="s">
         <v>207</v>
@@ -7140,7 +7140,7 @@
         <v>118</v>
       </c>
       <c r="O14" s="46" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="P14" s="51" t="s">
         <v>207</v>
@@ -7155,7 +7155,7 @@
         <v>219</v>
       </c>
       <c r="T14" s="49" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="U14" s="48" t="s">
         <v>228</v>
@@ -7181,7 +7181,7 @@
       </c>
       <c r="F15" s="46"/>
       <c r="G15" s="59" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="H15" s="55">
         <v>13</v>
@@ -7190,7 +7190,7 @@
         <v>208</v>
       </c>
       <c r="J15" s="61" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="K15" s="40" t="s">
         <v>208</v>
@@ -7218,7 +7218,7 @@
         <v>270</v>
       </c>
       <c r="T15" s="45" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="U15" s="44" t="s">
         <v>272</v>
@@ -7253,7 +7253,7 @@
         <v>207</v>
       </c>
       <c r="J16" s="61" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="K16" s="40" t="s">
         <v>208</v>
@@ -7281,7 +7281,7 @@
         <v>270</v>
       </c>
       <c r="T16" s="45" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="U16" s="44" t="s">
         <v>272</v>
@@ -7307,7 +7307,7 @@
         <v>255</v>
       </c>
       <c r="G17" s="38" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H17" s="55">
         <v>15</v>
@@ -7375,7 +7375,7 @@
         <v>208</v>
       </c>
       <c r="J18" s="61" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="K18" s="40" t="s">
         <v>207</v>
@@ -7386,7 +7386,7 @@
       <c r="M18" s="34"/>
       <c r="N18" s="34"/>
       <c r="O18" s="46" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="P18" s="51" t="s">
         <v>207</v>
@@ -7429,7 +7429,7 @@
       </c>
       <c r="F19" s="46"/>
       <c r="G19" s="38" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H19" s="55">
         <v>17</v>
@@ -7438,7 +7438,7 @@
         <v>208</v>
       </c>
       <c r="J19" s="61" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="K19" s="40" t="s">
         <v>208</v>
@@ -7464,7 +7464,7 @@
         <v>219</v>
       </c>
       <c r="T19" s="47" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="U19" s="47" t="s">
         <v>228</v>
@@ -7503,7 +7503,7 @@
         <v>208</v>
       </c>
       <c r="J20" s="61" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="K20" s="40" t="s">
         <v>208</v>
@@ -7531,7 +7531,7 @@
         <v>270</v>
       </c>
       <c r="T20" s="45" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="U20" s="44" t="s">
         <v>272</v>
@@ -7622,16 +7622,16 @@
       <c r="E22" s="37"/>
       <c r="F22" s="46"/>
       <c r="G22" s="59" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="H22" s="55">
         <v>20</v>
       </c>
       <c r="I22" s="55" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="J22" s="61" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="K22" s="40" t="s">
         <v>208</v>
@@ -7644,7 +7644,7 @@
       </c>
       <c r="N22" s="34"/>
       <c r="O22" s="57" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P22" s="51" t="s">
         <v>208</v>
@@ -7705,7 +7705,7 @@
         <v>103</v>
       </c>
       <c r="O23" s="46" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="P23" s="51" t="s">
         <v>207</v>
@@ -7720,7 +7720,7 @@
         <v>270</v>
       </c>
       <c r="T23" s="45" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="U23" s="44" t="s">
         <v>272</v>
@@ -7755,7 +7755,7 @@
         <v>208</v>
       </c>
       <c r="J24" s="61" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="K24" s="40" t="s">
         <v>208</v>
@@ -7768,7 +7768,7 @@
         <v>143</v>
       </c>
       <c r="O24" s="46" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="P24" s="51" t="s">
         <v>207</v>
@@ -7783,7 +7783,7 @@
         <v>270</v>
       </c>
       <c r="T24" s="45" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="U24" s="44" t="s">
         <v>272</v>
@@ -7809,7 +7809,7 @@
       <c r="E25" s="37"/>
       <c r="F25" s="46"/>
       <c r="G25" s="59" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H25" s="55">
         <v>23</v>
@@ -7818,7 +7818,7 @@
         <v>208</v>
       </c>
       <c r="J25" s="61" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="K25" s="40" t="s">
         <v>208</v>
@@ -7831,7 +7831,7 @@
         <v>139</v>
       </c>
       <c r="O25" s="46" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="P25" s="51" t="s">
         <v>208</v>
@@ -7846,7 +7846,7 @@
         <v>270</v>
       </c>
       <c r="T25" s="45" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="U25" s="44" t="s">
         <v>272</v>
@@ -7872,7 +7872,7 @@
       </c>
       <c r="F26" s="46"/>
       <c r="G26" s="38" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H26" s="55">
         <v>24</v>
@@ -7881,7 +7881,7 @@
         <v>208</v>
       </c>
       <c r="J26" s="61" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="K26" s="40" t="s">
         <v>208</v>
@@ -7909,7 +7909,7 @@
         <v>270</v>
       </c>
       <c r="T26" s="45" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="U26" s="44" t="s">
         <v>272</v>
@@ -7935,7 +7935,7 @@
       <c r="E27" s="37"/>
       <c r="F27" s="46"/>
       <c r="G27" s="59" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H27" s="55">
         <v>25</v>
@@ -7996,7 +7996,7 @@
       <c r="E28" s="37"/>
       <c r="F28" s="46"/>
       <c r="G28" s="38" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H28" s="55">
         <v>26</v>
@@ -8005,7 +8005,7 @@
         <v>208</v>
       </c>
       <c r="J28" s="61" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K28" s="40" t="s">
         <v>207</v>
@@ -8016,7 +8016,7 @@
       <c r="M28" s="34"/>
       <c r="N28" s="34"/>
       <c r="O28" s="46" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="P28" s="51" t="s">
         <v>207</v>
@@ -8028,13 +8028,13 @@
         <v>210</v>
       </c>
       <c r="S28" s="48" t="s">
+        <v>312</v>
+      </c>
+      <c r="T28" s="49" t="s">
         <v>313</v>
       </c>
-      <c r="T28" s="49" t="s">
+      <c r="U28" s="48" t="s">
         <v>314</v>
-      </c>
-      <c r="U28" s="48" t="s">
-        <v>315</v>
       </c>
       <c r="X28" s="33" t="s">
         <v>202</v>
@@ -8057,7 +8057,7 @@
       <c r="E29" s="37"/>
       <c r="F29" s="46"/>
       <c r="G29" s="59" t="s">
-        <v>289</v>
+        <v>352</v>
       </c>
       <c r="H29" s="55">
         <v>27</v>
@@ -8066,7 +8066,7 @@
         <v>208</v>
       </c>
       <c r="J29" s="61" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="K29" s="40" t="s">
         <v>208</v>
@@ -8079,7 +8079,7 @@
         <v>120</v>
       </c>
       <c r="O29" s="46" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="P29" s="51" t="s">
         <v>207</v>
@@ -8094,7 +8094,7 @@
         <v>270</v>
       </c>
       <c r="T29" s="45" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="U29" s="44" t="s">
         <v>272</v>
@@ -8220,14 +8220,14 @@
       <c r="E32" s="37"/>
       <c r="F32" s="46"/>
       <c r="G32" s="59" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="H32" s="55">
         <v>30</v>
       </c>
       <c r="I32" s="54"/>
       <c r="J32" s="61" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="K32" s="40"/>
       <c r="L32" s="33" t="s">
@@ -8483,104 +8483,104 @@
       <c r="Y41" s="38"/>
     </row>
     <row r="42" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A42" s="90"/>
-      <c r="B42" s="77"/>
-      <c r="C42" s="94"/>
+      <c r="A42" s="64"/>
+      <c r="B42" s="67"/>
+      <c r="C42" s="70"/>
       <c r="D42" s="36"/>
       <c r="E42" s="37"/>
       <c r="F42" s="36"/>
-      <c r="G42" s="68"/>
+      <c r="G42" s="97"/>
       <c r="H42" s="39"/>
-      <c r="I42" s="68"/>
-      <c r="J42" s="69"/>
-      <c r="K42" s="97"/>
-      <c r="L42" s="67"/>
-      <c r="M42" s="64"/>
-      <c r="N42" s="64"/>
-      <c r="O42" s="89"/>
-      <c r="P42" s="100"/>
+      <c r="I42" s="97"/>
+      <c r="J42" s="98"/>
+      <c r="K42" s="73"/>
+      <c r="L42" s="62"/>
+      <c r="M42" s="94"/>
+      <c r="N42" s="94"/>
+      <c r="O42" s="63"/>
+      <c r="P42" s="76"/>
       <c r="Q42" s="41"/>
       <c r="R42" s="43"/>
       <c r="S42" s="44"/>
       <c r="T42" s="45"/>
       <c r="U42" s="44"/>
-      <c r="X42" s="67"/>
-      <c r="Y42" s="67"/>
+      <c r="X42" s="62"/>
+      <c r="Y42" s="62"/>
     </row>
     <row r="43" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A43" s="91"/>
-      <c r="B43" s="93"/>
-      <c r="C43" s="95"/>
+      <c r="A43" s="65"/>
+      <c r="B43" s="68"/>
+      <c r="C43" s="71"/>
       <c r="D43" s="36"/>
       <c r="E43" s="37"/>
       <c r="F43" s="36"/>
-      <c r="G43" s="68"/>
+      <c r="G43" s="97"/>
       <c r="H43" s="39"/>
-      <c r="I43" s="68"/>
-      <c r="J43" s="69"/>
-      <c r="K43" s="98"/>
-      <c r="L43" s="67"/>
-      <c r="M43" s="65"/>
-      <c r="N43" s="65"/>
-      <c r="O43" s="89"/>
-      <c r="P43" s="101"/>
+      <c r="I43" s="97"/>
+      <c r="J43" s="98"/>
+      <c r="K43" s="74"/>
+      <c r="L43" s="62"/>
+      <c r="M43" s="95"/>
+      <c r="N43" s="95"/>
+      <c r="O43" s="63"/>
+      <c r="P43" s="77"/>
       <c r="Q43" s="41"/>
       <c r="R43" s="43"/>
       <c r="S43" s="44"/>
       <c r="T43" s="45"/>
       <c r="U43" s="44"/>
-      <c r="X43" s="67"/>
-      <c r="Y43" s="67"/>
+      <c r="X43" s="62"/>
+      <c r="Y43" s="62"/>
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A44" s="91"/>
-      <c r="B44" s="93"/>
-      <c r="C44" s="95"/>
+      <c r="A44" s="65"/>
+      <c r="B44" s="68"/>
+      <c r="C44" s="71"/>
       <c r="D44" s="36"/>
       <c r="E44" s="37"/>
       <c r="F44" s="36"/>
-      <c r="G44" s="68"/>
+      <c r="G44" s="97"/>
       <c r="H44" s="39"/>
-      <c r="I44" s="68"/>
-      <c r="J44" s="69"/>
-      <c r="K44" s="98"/>
-      <c r="L44" s="67"/>
-      <c r="M44" s="65"/>
-      <c r="N44" s="65"/>
-      <c r="O44" s="89"/>
-      <c r="P44" s="101"/>
+      <c r="I44" s="97"/>
+      <c r="J44" s="98"/>
+      <c r="K44" s="74"/>
+      <c r="L44" s="62"/>
+      <c r="M44" s="95"/>
+      <c r="N44" s="95"/>
+      <c r="O44" s="63"/>
+      <c r="P44" s="77"/>
       <c r="Q44" s="41"/>
       <c r="R44" s="43"/>
       <c r="S44" s="44"/>
       <c r="T44" s="45"/>
       <c r="U44" s="44"/>
-      <c r="X44" s="67"/>
-      <c r="Y44" s="67"/>
+      <c r="X44" s="62"/>
+      <c r="Y44" s="62"/>
     </row>
     <row r="45" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A45" s="92"/>
-      <c r="B45" s="78"/>
-      <c r="C45" s="96"/>
+      <c r="A45" s="66"/>
+      <c r="B45" s="69"/>
+      <c r="C45" s="72"/>
       <c r="D45" s="36"/>
       <c r="E45" s="37"/>
       <c r="F45" s="36"/>
-      <c r="G45" s="68"/>
+      <c r="G45" s="97"/>
       <c r="H45" s="39"/>
-      <c r="I45" s="68"/>
-      <c r="J45" s="69"/>
-      <c r="K45" s="99"/>
-      <c r="L45" s="67"/>
-      <c r="M45" s="66"/>
-      <c r="N45" s="66"/>
-      <c r="O45" s="89"/>
-      <c r="P45" s="102"/>
+      <c r="I45" s="97"/>
+      <c r="J45" s="98"/>
+      <c r="K45" s="75"/>
+      <c r="L45" s="62"/>
+      <c r="M45" s="96"/>
+      <c r="N45" s="96"/>
+      <c r="O45" s="63"/>
+      <c r="P45" s="78"/>
       <c r="Q45" s="41"/>
       <c r="R45" s="43"/>
       <c r="S45" s="44"/>
       <c r="T45" s="45"/>
       <c r="U45" s="44"/>
-      <c r="X45" s="67"/>
-      <c r="Y45" s="67"/>
+      <c r="X45" s="62"/>
+      <c r="Y45" s="62"/>
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A46" s="30"/>
@@ -9509,29 +9509,6 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="Y42:Y45"/>
-    <mergeCell ref="O42:O45"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="B42:B45"/>
-    <mergeCell ref="C42:C45"/>
-    <mergeCell ref="X42:X45"/>
-    <mergeCell ref="K42:K45"/>
-    <mergeCell ref="P42:P45"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="P1:P2"/>
     <mergeCell ref="M42:M45"/>
     <mergeCell ref="N42:N45"/>
@@ -9543,6 +9520,29 @@
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="M1:N1"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="Y42:Y45"/>
+    <mergeCell ref="O42:O45"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="B42:B45"/>
+    <mergeCell ref="C42:C45"/>
+    <mergeCell ref="X42:X45"/>
+    <mergeCell ref="K42:K45"/>
+    <mergeCell ref="P42:P45"/>
   </mergeCells>
   <dataValidations count="9">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A46">

</xml_diff>